<commit_message>
Finish first version of software specification
</commit_message>
<xml_diff>
--- a/docs/Cronograma.xlsx
+++ b/docs/Cronograma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cnpemcamp-my.sharepoint.com/personal/gabriel_brunheira_lnls_br/Documents/Pessoal/UNICAMP/IM420X/Projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.brunheira\Git\pessoal\project-reggae\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{B5CDC92F-0C90-4003-9E24-C5A14E85A924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A51AF3B-CA01-4E19-A25A-A5F629644CEE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E80A45-3744-420C-B36D-EF26F71B0676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BC82D3A-C5F0-42FE-AE72-D21310DA2092}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2BC82D3A-C5F0-42FE-AE72-D21310DA2092}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Finalizar projeto de hardware</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Programação e teste de periféricos</t>
   </si>
   <si>
-    <t>Detalhamento do projeto de software: definição do uso de periféricos e componentes do RTOS, especificação da memória de registro de dados e protocolo de comunicação com PC</t>
-  </si>
-  <si>
     <t>Especificação da aplicação em Python</t>
   </si>
   <si>
@@ -75,13 +72,28 @@
   </si>
   <si>
     <t>Semana / último dia</t>
+  </si>
+  <si>
+    <t>Detalhamento do projeto de software: definição do uso de periféricos e componentes do RTOS, especificação da memória de registro de dados</t>
+  </si>
+  <si>
+    <t>Planejado</t>
+  </si>
+  <si>
+    <t>Executado</t>
+  </si>
+  <si>
+    <t>Iniciado</t>
+  </si>
+  <si>
+    <t>Atrasado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,22 +103,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -133,8 +129,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,8 +179,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -356,11 +382,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -371,7 +412,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -380,71 +454,59 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,369 +842,392 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4A0763-B499-4DB1-9D28-D73FC2819120}">
-  <dimension ref="B3:J28"/>
+  <dimension ref="C3:N35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B20"/>
+      <selection activeCell="M7" sqref="M7:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="90" style="1" customWidth="1"/>
-    <col min="3" max="10" width="8.7109375" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="90" style="1" customWidth="1"/>
+    <col min="4" max="11" width="8.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="3"/>
+    <col min="13" max="13" width="9.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="34" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:10" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="s">
+    <row r="3" spans="3:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:14" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
       <c r="J4" s="25"/>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="27"/>
-      <c r="C5" s="14">
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" spans="3:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C5" s="28"/>
+      <c r="D5" s="15">
         <v>1</v>
       </c>
-      <c r="D5" s="15">
+      <c r="E5" s="16">
         <v>2</v>
       </c>
-      <c r="E5" s="15">
+      <c r="F5" s="16">
         <v>3</v>
       </c>
-      <c r="F5" s="15">
+      <c r="G5" s="16">
         <v>4</v>
       </c>
-      <c r="G5" s="15">
+      <c r="H5" s="16">
         <v>5</v>
       </c>
-      <c r="H5" s="15">
+      <c r="I5" s="16">
         <v>6</v>
       </c>
-      <c r="I5" s="15">
+      <c r="J5" s="16">
         <v>7</v>
       </c>
-      <c r="J5" s="16">
+      <c r="K5" s="17">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="28"/>
-      <c r="C6" s="17">
+    <row r="6" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="29"/>
+      <c r="D6" s="18">
         <v>45573</v>
       </c>
-      <c r="D6" s="18">
+      <c r="E6" s="19">
         <v>45580</v>
       </c>
-      <c r="E6" s="18">
+      <c r="F6" s="19">
         <v>45587</v>
       </c>
-      <c r="F6" s="18">
+      <c r="G6" s="19">
         <v>45594</v>
       </c>
-      <c r="G6" s="18">
+      <c r="H6" s="19">
         <v>45601</v>
       </c>
-      <c r="H6" s="18">
+      <c r="I6" s="19">
         <v>45608</v>
       </c>
-      <c r="I6" s="18">
+      <c r="J6" s="19">
         <v>45615</v>
       </c>
-      <c r="J6" s="19">
+      <c r="K6" s="20">
         <v>45622</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+    <row r="7" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="8"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="13"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="23"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C9" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="22"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="8"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="23"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="22"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="23"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="J12" s="8"/>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="22"/>
-      <c r="C14" s="8"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="23"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="5"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="22" t="s">
+        <v>3</v>
+      </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="22"/>
-      <c r="C16" s="8"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="23"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="5"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C17" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="22"/>
-      <c r="C18" s="8"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="23"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="G18" s="21"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="5"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C19" s="22" t="s">
+        <v>5</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="4"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22"/>
-      <c r="C20" s="8"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="23"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="G20" s="21"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="5"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C21" s="22" t="s">
+        <v>6</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="4"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="22"/>
-      <c r="C22" s="8"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="23"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="5"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="22" t="s">
+        <v>7</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22"/>
-      <c r="C24" s="8"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="23"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="5"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="9"/>
+    </row>
+    <row r="25" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C25" s="22" t="s">
+        <v>8</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="22"/>
-      <c r="C26" s="8"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="23"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="5"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C27" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="22"/>
-      <c r="C28" s="8"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="23"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="9"/>
-    </row>
+      <c r="J28" s="8"/>
+      <c r="K28" s="9"/>
+    </row>
+    <row r="32" spans="3:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Include lib and proof-of-concepts of OLED display
</commit_message>
<xml_diff>
--- a/docs/Cronograma.xlsx
+++ b/docs/Cronograma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.brunheira\Git\pessoal\project-reggae\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E80A45-3744-420C-B36D-EF26F71B0676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BF857D-B980-428F-B7D9-714BC2FE99F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2BC82D3A-C5F0-42FE-AE72-D21310DA2092}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BC82D3A-C5F0-42FE-AE72-D21310DA2092}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -466,47 +466,47 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,7 +845,7 @@
   <dimension ref="C3:N35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:N10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -855,28 +855,28 @@
     <col min="4" max="11" width="8.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="3"/>
     <col min="13" max="13" width="9.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="34" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="26" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:14" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="26"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
     </row>
     <row r="5" spans="3:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="C5" s="28"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="15">
         <v>1</v>
       </c>
@@ -903,7 +903,7 @@
       </c>
     </row>
     <row r="6" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="29"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="18">
         <v>45573</v>
       </c>
@@ -930,7 +930,7 @@
       </c>
     </row>
     <row r="7" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="34" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="11"/>
@@ -941,13 +941,13 @@
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="13"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="35" t="s">
+      <c r="M7" s="22"/>
+      <c r="N7" s="27" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="23"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="8"/>
@@ -956,13 +956,13 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="9"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="35" t="s">
+      <c r="M8" s="23"/>
+      <c r="N8" s="27" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="34" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="5"/>
@@ -973,13 +973,13 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="35" t="s">
+      <c r="M9" s="24"/>
+      <c r="N9" s="27" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="23"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="8"/>
       <c r="E10" s="14"/>
       <c r="F10" s="8"/>
@@ -988,13 +988,13 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="35" t="s">
+      <c r="M10" s="25"/>
+      <c r="N10" s="27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="34" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="5"/>
@@ -1007,7 +1007,7 @@
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="23"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="8"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -1018,7 +1018,7 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="5"/>
@@ -1031,18 +1031,18 @@
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="23"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="8"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="34" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="5"/>
@@ -1055,7 +1055,7 @@
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="3:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="23"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="7"/>
@@ -1066,7 +1066,7 @@
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="34" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="5"/>
@@ -1079,7 +1079,7 @@
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="23"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1090,7 +1090,7 @@
       <c r="K18" s="9"/>
     </row>
     <row r="19" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="34" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="5"/>
@@ -1103,7 +1103,7 @@
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="23"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1114,7 +1114,7 @@
       <c r="K20" s="9"/>
     </row>
     <row r="21" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="34" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="5"/>
@@ -1127,7 +1127,7 @@
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="23"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1138,7 +1138,7 @@
       <c r="K22" s="9"/>
     </row>
     <row r="23" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="34" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="5"/>
@@ -1151,7 +1151,7 @@
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="23"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -1162,7 +1162,7 @@
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="34" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="5"/>
@@ -1175,7 +1175,7 @@
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="23"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -1186,7 +1186,7 @@
       <c r="K26" s="9"/>
     </row>
     <row r="27" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="34" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="5"/>
@@ -1199,7 +1199,7 @@
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="23"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -1215,11 +1215,6 @@
     <row r="35" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D4:K4"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C27:C28"/>
@@ -1228,6 +1223,11 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>